<commit_message>
Aalmeen changes merged with latest and calling added from App
</commit_message>
<xml_diff>
--- a/Automation-UserCMD/TestData/Outputs/ContentOutput.xlsx
+++ b/Automation-UserCMD/TestData/Outputs/ContentOutput.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Content" sheetId="1" r:id="R9c6f378b68484450"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Content" sheetId="1" r:id="Ra81fb6ea25fc4b65"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -66,7 +66,7 @@
         <x:v/>
       </x:c>
       <x:c r="H2" t="str">
-        <x:v>11/20/2015</x:v>
+        <x:v>42328.6278935185</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
@@ -92,7 +92,7 @@
         <x:v>arun.kesavan</x:v>
       </x:c>
       <x:c r="H3" t="str">
-        <x:v>11/20/2015</x:v>
+        <x:v>42328.6278935185</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
@@ -118,7 +118,7 @@
         <x:v>manualsubmission</x:v>
       </x:c>
       <x:c r="H4" t="str">
-        <x:v>12/1/2015</x:v>
+        <x:v>42339.942037037</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -144,7 +144,7 @@
         <x:v>Learning Analytics</x:v>
       </x:c>
       <x:c r="H5" t="str">
-        <x:v>11/18/2015</x:v>
+        <x:v>42326.942037037</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
@@ -152,25 +152,25 @@
         <x:v>update</x:v>
       </x:c>
       <x:c r="B6" t="str">
-        <x:v>1934288</x:v>
+        <x:v>edf6eed1-40f2-469c-ae7e-f6e0de90167a</x:v>
       </x:c>
       <x:c r="C6" t="str">
-        <x:v>Composite</x:v>
+        <x:v>Read, Write, Learn</x:v>
       </x:c>
       <x:c r="D6" t="str">
-        <x:v>question</x:v>
+        <x:v>Episode</x:v>
       </x:c>
       <x:c r="E6" t="str">
         <x:v/>
       </x:c>
       <x:c r="F6" t="str">
-        <x:v>[{"id":"c9523d19-ee08-44b7-b3a7-ece580db8a83","subtype":null,"type":"assessment"}]</x:v>
+        <x:v>[{"id":"40d2a3eb-40f2-4e10-806c-50f310db5957","subtype":null,"type":"Unit"}]</x:v>
       </x:c>
       <x:c r="G6" t="str">
-        <x:v/>
+        <x:v>Learning Analytics</x:v>
       </x:c>
       <x:c r="H6" t="str">
-        <x:v>11/20/2015</x:v>
+        <x:v>42326.942037037</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
@@ -178,25 +178,25 @@
         <x:v>update</x:v>
       </x:c>
       <x:c r="B7" t="str">
-        <x:v>1934291</x:v>
+        <x:v>40d2a3eb-40f2-4e10-806c-50f310db5957</x:v>
       </x:c>
       <x:c r="C7" t="str">
-        <x:v>Composite</x:v>
+        <x:v>Read, Write, Learn</x:v>
       </x:c>
       <x:c r="D7" t="str">
-        <x:v>question</x:v>
+        <x:v>Unit</x:v>
       </x:c>
       <x:c r="E7" t="str">
         <x:v/>
       </x:c>
       <x:c r="F7" t="str">
-        <x:v>[{"id":"c9523d19-ee08-44b7-b3a7-ece580db8a83","subtype":null,"type":"assessment"}]</x:v>
+        <x:v/>
       </x:c>
       <x:c r="G7" t="str">
-        <x:v/>
+        <x:v>Learning Analytics</x:v>
       </x:c>
       <x:c r="H7" t="str">
-        <x:v>11/20/2015</x:v>
+        <x:v>42326.942037037</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
@@ -204,7 +204,7 @@
         <x:v>update</x:v>
       </x:c>
       <x:c r="B8" t="str">
-        <x:v>1934293</x:v>
+        <x:v>1934288</x:v>
       </x:c>
       <x:c r="C8" t="str">
         <x:v>Composite</x:v>
@@ -222,7 +222,7 @@
         <x:v/>
       </x:c>
       <x:c r="H8" t="str">
-        <x:v>11/20/2015</x:v>
+        <x:v>42328.6303356482</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
@@ -230,25 +230,25 @@
         <x:v>update</x:v>
       </x:c>
       <x:c r="B9" t="str">
-        <x:v>c9523d19-ee08-44b7-b3a7-ece580db8a83</x:v>
+        <x:v>1934291</x:v>
       </x:c>
       <x:c r="C9" t="str">
-        <x:v>1.1 Unit Accomplishments</x:v>
+        <x:v>Composite</x:v>
       </x:c>
       <x:c r="D9" t="str">
-        <x:v>assessment</x:v>
+        <x:v>question</x:v>
       </x:c>
       <x:c r="E9" t="str">
         <x:v/>
       </x:c>
       <x:c r="F9" t="str">
-        <x:v/>
+        <x:v>[{"id":"c9523d19-ee08-44b7-b3a7-ece580db8a83","subtype":null,"type":"assessment"}]</x:v>
       </x:c>
       <x:c r="G9" t="str">
-        <x:v>narendra.nikam</x:v>
+        <x:v/>
       </x:c>
       <x:c r="H9" t="str">
-        <x:v>11/20/2015</x:v>
+        <x:v>42328.6304166667</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
@@ -256,25 +256,77 @@
         <x:v>update</x:v>
       </x:c>
       <x:c r="B10" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="C10" t="str">
+        <x:v>Composite</x:v>
+      </x:c>
+      <x:c r="D10" t="str">
+        <x:v>question</x:v>
+      </x:c>
+      <x:c r="E10" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="F10" t="str">
+        <x:v>[{"id":"c9523d19-ee08-44b7-b3a7-ece580db8a83","subtype":null,"type":"assessment"}]</x:v>
+      </x:c>
+      <x:c r="G10" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="H10" t="str">
+        <x:v>42328.6305092593</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11">
+      <x:c r="A11" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B11" t="str">
+        <x:v>c9523d19-ee08-44b7-b3a7-ece580db8a83</x:v>
+      </x:c>
+      <x:c r="C11" t="str">
+        <x:v>1.1 Unit Accomplishments</x:v>
+      </x:c>
+      <x:c r="D11" t="str">
+        <x:v>assessment</x:v>
+      </x:c>
+      <x:c r="E11" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="F11" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="G11" t="str">
+        <x:v>narendra.nikam</x:v>
+      </x:c>
+      <x:c r="H11" t="str">
+        <x:v>42328.6303356482</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12">
+      <x:c r="A12" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B12" t="str">
         <x:v>40d2a3eb-40f2-4e10-806c-50f310db5957</x:v>
       </x:c>
-      <x:c r="C10" t="str">
+      <x:c r="C12" t="str">
         <x:v>Read, Write, Learn</x:v>
       </x:c>
-      <x:c r="D10" t="str">
+      <x:c r="D12" t="str">
         <x:v>Unit</x:v>
       </x:c>
-      <x:c r="E10" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="F10" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="G10" t="str">
+      <x:c r="E12" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="F12" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="G12" t="str">
         <x:v>manualsubmission</x:v>
       </x:c>
-      <x:c r="H10" t="str">
-        <x:v>12/1/2015</x:v>
+      <x:c r="H12" t="str">
+        <x:v>42339.942037037</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>